<commit_message>
Mise en place des bulletins semestriels
</commit_message>
<xml_diff>
--- a/excel/M2-S3/M2-S3-MAPI.xlsx
+++ b/excel/M2-S3/M2-S3-MAPI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndyVESPUCE\bulletin-espi\backend\excel\M2-S3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3664A7C-F0AB-47FE-AB27-1C7AE63F027B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C65BDB-2A22-4143-BD12-8A3DD935D50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,21 +36,6 @@
     <t>Economie immobilière II</t>
   </si>
   <si>
-    <t>UE 3 - AMENAGEMENT &amp; URBANISME</t>
-  </si>
-  <si>
-    <t>Stratégies et aménagement des territoires I</t>
-  </si>
-  <si>
-    <t>UE 4 - COMPETENCES PROFESSIONNALISANTES</t>
-  </si>
-  <si>
-    <t>Communication digitale écrite orale</t>
-  </si>
-  <si>
-    <t>Immersion professionnelle</t>
-  </si>
-  <si>
     <t>Real Estate English</t>
   </si>
   <si>
@@ -66,21 +51,6 @@
     <t>UE SPE – MAPI</t>
   </si>
   <si>
-    <t>Acquisition et dissociation du foncier</t>
-  </si>
-  <si>
-    <t>Montage des opérations tertiaires</t>
-  </si>
-  <si>
-    <t>Aménagement et commande publique</t>
-  </si>
-  <si>
-    <t>Techniques du batiment</t>
-  </si>
-  <si>
-    <t>Réhabilitation et pathologies du batiment</t>
-  </si>
-  <si>
     <t>Code Apprenant</t>
   </si>
   <si>
@@ -112,6 +82,36 @@
   </si>
   <si>
     <t>Retards</t>
+  </si>
+  <si>
+    <t>UE 3 – Aménagement &amp; Urbanisme</t>
+  </si>
+  <si>
+    <t>UE 4 – Compétences Professionnalisantes</t>
+  </si>
+  <si>
+    <t>Immersion Professionnelle</t>
+  </si>
+  <si>
+    <t>Communication Digitale, Ecrite et Orale</t>
+  </si>
+  <si>
+    <t>Stratégies et Aménagement des Territoires I</t>
+  </si>
+  <si>
+    <t>Acquisition et Dissociation du Foncier</t>
+  </si>
+  <si>
+    <t>Techniques du Bâtiment</t>
+  </si>
+  <si>
+    <t>Réhabilitation et Pathologies du Bâtiment</t>
+  </si>
+  <si>
+    <t>Aménagement et Commande Publique</t>
+  </si>
+  <si>
+    <t>Montage des Opérations Tertiaires</t>
   </si>
 </sst>
 </file>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,49 +671,49 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
@@ -726,88 +726,88 @@
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">

</xml_diff>